<commit_message>
Modular inverter model aktarım çalışmaları.
</commit_message>
<xml_diff>
--- a/Simulation/analytical model/harmonic_components.xlsx
+++ b/Simulation/analytical model/harmonic_components.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mesutto\Desktop\github work\IMMD\Simulation\analytical model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\immdnew\Simulation\analytical model\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
   <si>
     <t>DC</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>IS-B</t>
+  </si>
+  <si>
+    <t>IDC</t>
   </si>
 </sst>
 </file>
@@ -138,13 +141,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -185,7 +185,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -467,13 +473,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:S25"/>
+  <dimension ref="C1:S36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C1" s="19" t="s">
@@ -482,92 +491,92 @@
       <c r="D1" s="19"/>
       <c r="E1" s="19"/>
       <c r="F1" s="19"/>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3" t="s">
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3" t="s">
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-    </row>
-    <row r="2" spans="3:19" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="4"/>
-      <c r="D2" s="4" t="s">
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+    </row>
+    <row r="2" spans="3:19" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="4">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="3">
         <v>0.5</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="K2" s="4">
+      <c r="I2" s="3"/>
+      <c r="J2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="3">
         <v>0.5</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="N2" s="4">
+      <c r="L2" s="3"/>
+      <c r="M2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="3">
         <v>0.5</v>
       </c>
-      <c r="O2" s="4"/>
+      <c r="O2" s="3"/>
     </row>
     <row r="3" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="14">
         <v>197</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="15">
         <f>D3/270</f>
         <v>0.72962962962962963</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="16">
         <v>36.5</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="15">
+      <c r="H3" s="14">
         <v>0.42249999999999999</v>
       </c>
-      <c r="I3" s="17">
+      <c r="I3" s="16">
         <v>6.5</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="15">
+      <c r="K3" s="14">
         <v>0.42230000000000001</v>
       </c>
-      <c r="L3" s="17">
+      <c r="L3" s="16">
         <v>246.5</v>
       </c>
-      <c r="M3" s="14" t="s">
+      <c r="M3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="N3" s="15">
+      <c r="N3" s="14">
         <v>0.42220000000000002</v>
       </c>
-      <c r="O3" s="17">
+      <c r="O3" s="16">
         <v>126.5</v>
       </c>
       <c r="Q3">
@@ -584,59 +593,59 @@
       </c>
     </row>
     <row r="4" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C4" s="4"/>
-      <c r="D4" s="5"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="4"/>
       <c r="E4" s="1"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="5"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="4"/>
       <c r="I4" s="2"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="5"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="4"/>
       <c r="L4" s="2"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="5"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="4"/>
       <c r="O4" s="2"/>
     </row>
     <row r="5" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C5" s="10">
+      <c r="C5" s="9">
         <v>9900</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="10">
         <v>56.4818</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="11">
         <f>D5/270</f>
         <v>0.20919185185185185</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="12">
         <v>103</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="9">
         <v>9900</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="10">
         <v>0.1205</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5" s="12">
         <v>77</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="9">
         <v>9900</v>
       </c>
-      <c r="K5" s="11">
+      <c r="K5" s="10">
         <v>0.12089999999999999</v>
       </c>
-      <c r="L5" s="13">
+      <c r="L5" s="12">
         <v>-43</v>
       </c>
-      <c r="M5" s="10">
+      <c r="M5" s="9">
         <v>9900</v>
       </c>
-      <c r="N5" s="11">
+      <c r="N5" s="10">
         <v>0.12089999999999999</v>
       </c>
-      <c r="O5" s="13">
+      <c r="O5" s="12">
         <v>196</v>
       </c>
       <c r="Q5">
@@ -653,37 +662,37 @@
       </c>
     </row>
     <row r="6" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>10000</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="6">
+      <c r="D6" s="6"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="5">
         <v>10000</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="6">
         <v>0.38569999999999999</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="7">
         <v>90</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="5">
         <v>10000</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="6">
         <v>0.38579999999999998</v>
       </c>
-      <c r="L6" s="8">
+      <c r="L6" s="7">
         <v>90</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M6" s="5">
         <v>10000</v>
       </c>
-      <c r="N6" s="7">
+      <c r="N6" s="6">
         <v>0.38590000000000002</v>
       </c>
-      <c r="O6" s="8">
+      <c r="O6" s="7">
         <v>90</v>
       </c>
       <c r="Q6">
@@ -700,44 +709,44 @@
       </c>
     </row>
     <row r="7" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C7" s="10">
+      <c r="C7" s="9">
         <v>10100</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="10">
         <v>56.4358</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="11">
         <f>D7/270</f>
         <v>0.20902148148148147</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="12">
         <v>69</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="9">
         <v>10100</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="10">
         <v>0.1208</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I7" s="12">
         <v>103</v>
       </c>
-      <c r="J7" s="10">
+      <c r="J7" s="9">
         <v>10100</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K7" s="10">
         <v>0.1207</v>
       </c>
-      <c r="L7" s="13">
+      <c r="L7" s="12">
         <v>223</v>
       </c>
-      <c r="M7" s="10">
+      <c r="M7" s="9">
         <v>10100</v>
       </c>
-      <c r="N7" s="11">
+      <c r="N7" s="10">
         <v>0.1207</v>
       </c>
-      <c r="O7" s="13">
+      <c r="O7" s="12">
         <v>-16</v>
       </c>
       <c r="Q7">
@@ -754,52 +763,52 @@
       </c>
     </row>
     <row r="8" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="4"/>
       <c r="E8" s="1"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="5"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="4"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="5"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="4"/>
       <c r="L8" s="2"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="5"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="4"/>
       <c r="O8" s="2"/>
     </row>
     <row r="9" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>19850</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="6">
+      <c r="D9" s="6"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="5">
         <v>19850</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="6">
         <v>7.8299999999999995E-2</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9" s="7">
         <v>-19</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="5">
         <v>19850</v>
       </c>
-      <c r="K9" s="7">
+      <c r="K9" s="6">
         <v>7.8399999999999997E-2</v>
       </c>
-      <c r="L9" s="8">
+      <c r="L9" s="7">
         <v>-20</v>
       </c>
-      <c r="M9" s="6">
+      <c r="M9" s="5">
         <v>19850</v>
       </c>
-      <c r="N9" s="7">
+      <c r="N9" s="6">
         <v>7.8100000000000003E-2</v>
       </c>
-      <c r="O9" s="8">
+      <c r="O9" s="7">
         <v>-20</v>
       </c>
       <c r="Q9">
@@ -816,44 +825,44 @@
       </c>
     </row>
     <row r="10" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C10" s="10">
+      <c r="C10" s="9">
         <v>19950</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="10">
         <v>67.620199999999997</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="11">
         <f>D10/270</f>
         <v>0.25044518518518516</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="12">
         <v>-43</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="9">
         <v>19950</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="10">
         <v>0.14510000000000001</v>
       </c>
-      <c r="I10" s="13">
+      <c r="I10" s="12">
         <v>-6</v>
       </c>
-      <c r="J10" s="10">
+      <c r="J10" s="9">
         <v>19950</v>
       </c>
-      <c r="K10" s="11">
+      <c r="K10" s="10">
         <v>0.14480000000000001</v>
       </c>
-      <c r="L10" s="13">
+      <c r="L10" s="12">
         <v>113</v>
       </c>
-      <c r="M10" s="10">
+      <c r="M10" s="9">
         <v>19950</v>
       </c>
-      <c r="N10" s="11">
+      <c r="N10" s="10">
         <v>0.14480000000000001</v>
       </c>
-      <c r="O10" s="13">
+      <c r="O10" s="12">
         <v>233</v>
       </c>
       <c r="Q10">
@@ -870,44 +879,44 @@
       </c>
     </row>
     <row r="11" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C11" s="10">
+      <c r="C11" s="9">
         <v>20050</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="10">
         <v>67.704899999999995</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="11">
         <f>D11/270</f>
         <v>0.25075888888888886</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11" s="12">
         <v>209</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11" s="9">
         <v>20050</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="10">
         <v>0.14480000000000001</v>
       </c>
-      <c r="I11" s="13">
+      <c r="I11" s="12">
         <v>186</v>
       </c>
-      <c r="J11" s="10">
+      <c r="J11" s="9">
         <v>20050</v>
       </c>
-      <c r="K11" s="11">
+      <c r="K11" s="10">
         <v>0.14499999999999999</v>
       </c>
-      <c r="L11" s="13">
+      <c r="L11" s="12">
         <v>67</v>
       </c>
-      <c r="M11" s="10">
+      <c r="M11" s="9">
         <v>20050</v>
       </c>
-      <c r="N11" s="11">
+      <c r="N11" s="10">
         <v>0.14499999999999999</v>
       </c>
-      <c r="O11" s="13">
+      <c r="O11" s="12">
         <v>-53</v>
       </c>
       <c r="Q11">
@@ -924,37 +933,37 @@
       </c>
     </row>
     <row r="12" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>20150</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="6">
+      <c r="D12" s="6"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="5">
         <v>20150</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="6">
         <v>7.85E-2</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="7">
         <v>199</v>
       </c>
-      <c r="J12" s="6">
+      <c r="J12" s="5">
         <v>20150</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K12" s="6">
         <v>7.8299999999999995E-2</v>
       </c>
-      <c r="L12" s="8">
+      <c r="L12" s="7">
         <v>199</v>
       </c>
-      <c r="M12" s="6">
+      <c r="M12" s="5">
         <v>20150</v>
       </c>
-      <c r="N12" s="7">
+      <c r="N12" s="6">
         <v>7.8100000000000003E-2</v>
       </c>
-      <c r="O12" s="8">
+      <c r="O12" s="7">
         <v>199</v>
       </c>
       <c r="Q12">
@@ -971,65 +980,65 @@
       </c>
     </row>
     <row r="14" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3" t="s">
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3" t="s">
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="18"/>
     </row>
     <row r="15" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="G15" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
+      <c r="G15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
     </row>
     <row r="16" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="G16" s="14" t="s">
+      <c r="G16" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="H16" s="15">
+      <c r="H16" s="14">
         <v>11.744199999999999</v>
       </c>
-      <c r="I16" s="17">
+      <c r="I16" s="16">
         <v>-0.8</v>
       </c>
-      <c r="J16" s="14" t="s">
+      <c r="J16" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K16" s="15">
+      <c r="K16" s="14">
         <v>11.7676</v>
       </c>
-      <c r="L16" s="17">
+      <c r="L16" s="16">
         <v>239.7</v>
       </c>
-      <c r="M16" s="14" t="s">
+      <c r="M16" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="N16" s="15">
+      <c r="N16" s="14">
         <v>11.8529</v>
       </c>
-      <c r="O16" s="17">
+      <c r="O16" s="16">
         <v>119.3</v>
       </c>
       <c r="Q16">
@@ -1046,73 +1055,73 @@
       </c>
     </row>
     <row r="17" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G17" s="4"/>
-      <c r="H17" s="5"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="4"/>
       <c r="I17" s="2"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="5"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="4"/>
       <c r="L17" s="2"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="5"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="4"/>
       <c r="O17" s="2"/>
     </row>
     <row r="18" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G18" s="10">
+      <c r="G18" s="9">
         <v>9900</v>
       </c>
-      <c r="H18" s="11">
+      <c r="H18" s="10">
         <v>0.14949999999999999</v>
       </c>
-      <c r="I18" s="13">
+      <c r="I18" s="12">
         <v>-16.600000000000001</v>
       </c>
-      <c r="J18" s="10">
+      <c r="J18" s="9">
         <v>9900</v>
       </c>
-      <c r="K18" s="11">
+      <c r="K18" s="10">
         <v>0.14990000000000001</v>
       </c>
-      <c r="L18" s="13">
+      <c r="L18" s="12">
         <v>223.3</v>
       </c>
-      <c r="M18" s="10">
+      <c r="M18" s="9">
         <v>9900</v>
       </c>
-      <c r="N18" s="11">
+      <c r="N18" s="10">
         <v>0.1497</v>
       </c>
-      <c r="O18" s="13">
+      <c r="O18" s="12">
         <v>103.3</v>
       </c>
       <c r="Q18">
-        <f t="shared" ref="Q18:Q25" si="3">I18-L18</f>
+        <f t="shared" ref="Q18:Q20" si="3">I18-L18</f>
         <v>-239.9</v>
       </c>
       <c r="R18">
-        <f t="shared" ref="R18:R25" si="4">L18-O18</f>
+        <f t="shared" ref="R18:R20" si="4">L18-O18</f>
         <v>120.00000000000001</v>
       </c>
       <c r="S18">
-        <f t="shared" ref="S18:S25" si="5">O18-I18</f>
+        <f t="shared" ref="S18:S20" si="5">O18-I18</f>
         <v>119.9</v>
       </c>
     </row>
     <row r="19" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G19" s="6">
+      <c r="G19" s="5">
         <v>10000</v>
       </c>
-      <c r="H19" s="7"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="6">
+      <c r="H19" s="6"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="5">
         <v>10000</v>
       </c>
-      <c r="K19" s="7"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="6">
+      <c r="K19" s="6"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="5">
         <v>10000</v>
       </c>
-      <c r="N19" s="7"/>
-      <c r="O19" s="8"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="7"/>
       <c r="Q19">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -1127,31 +1136,31 @@
       </c>
     </row>
     <row r="20" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G20" s="10">
+      <c r="G20" s="9">
         <v>10100</v>
       </c>
-      <c r="H20" s="11">
+      <c r="H20" s="10">
         <v>0.14680000000000001</v>
       </c>
-      <c r="I20" s="13">
+      <c r="I20" s="12">
         <v>9.5</v>
       </c>
-      <c r="J20" s="10">
+      <c r="J20" s="9">
         <v>10100</v>
       </c>
-      <c r="K20" s="11">
+      <c r="K20" s="10">
         <v>0.14660000000000001</v>
       </c>
-      <c r="L20" s="13">
+      <c r="L20" s="12">
         <v>129.4</v>
       </c>
-      <c r="M20" s="10">
+      <c r="M20" s="9">
         <v>10100</v>
       </c>
-      <c r="N20" s="11">
+      <c r="N20" s="10">
         <v>0.14680000000000001</v>
       </c>
-      <c r="O20" s="13">
+      <c r="O20" s="12">
         <v>249.4</v>
       </c>
       <c r="Q20">
@@ -1168,32 +1177,32 @@
       </c>
     </row>
     <row r="21" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G21" s="4"/>
-      <c r="H21" s="5"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="4"/>
       <c r="I21" s="2"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="5"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="4"/>
       <c r="L21" s="2"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="5"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="4"/>
       <c r="O21" s="2"/>
     </row>
     <row r="22" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G22" s="6">
+      <c r="G22" s="5">
         <v>19850</v>
       </c>
-      <c r="H22" s="7"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="6">
+      <c r="H22" s="6"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="5">
         <v>19850</v>
       </c>
-      <c r="K22" s="7"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="6">
+      <c r="K22" s="6"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="5">
         <v>19850</v>
       </c>
-      <c r="N22" s="7"/>
-      <c r="O22" s="8"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="7"/>
       <c r="Q22">
         <f t="shared" ref="Q22:Q25" si="6">I22-L22</f>
         <v>0</v>
@@ -1208,31 +1217,31 @@
       </c>
     </row>
     <row r="23" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G23" s="10">
+      <c r="G23" s="9">
         <v>19950</v>
       </c>
-      <c r="H23" s="11">
+      <c r="H23" s="10">
         <v>8.9200000000000002E-2</v>
       </c>
-      <c r="I23" s="13">
+      <c r="I23" s="12">
         <v>256</v>
       </c>
-      <c r="J23" s="10">
+      <c r="J23" s="9">
         <v>19950</v>
       </c>
-      <c r="K23" s="11">
+      <c r="K23" s="10">
         <v>8.8900000000000007E-2</v>
       </c>
-      <c r="L23" s="13">
+      <c r="L23" s="12">
         <v>16.2</v>
       </c>
-      <c r="M23" s="10">
+      <c r="M23" s="9">
         <v>19950</v>
       </c>
-      <c r="N23" s="11">
+      <c r="N23" s="10">
         <v>8.9200000000000002E-2</v>
       </c>
-      <c r="O23" s="13">
+      <c r="O23" s="12">
         <v>136.1</v>
       </c>
       <c r="Q23">
@@ -1249,31 +1258,31 @@
       </c>
     </row>
     <row r="24" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G24" s="10">
+      <c r="G24" s="9">
         <v>20050</v>
       </c>
-      <c r="H24" s="11">
+      <c r="H24" s="10">
         <v>8.8599999999999998E-2</v>
       </c>
-      <c r="I24" s="13">
+      <c r="I24" s="12">
         <v>89</v>
       </c>
-      <c r="J24" s="10">
+      <c r="J24" s="9">
         <v>20050</v>
       </c>
-      <c r="K24" s="11">
+      <c r="K24" s="10">
         <v>8.8599999999999998E-2</v>
       </c>
-      <c r="L24" s="13">
+      <c r="L24" s="12">
         <v>-30.6</v>
       </c>
-      <c r="M24" s="10">
+      <c r="M24" s="9">
         <v>20050</v>
       </c>
-      <c r="N24" s="11">
+      <c r="N24" s="10">
         <v>8.8700000000000001E-2</v>
       </c>
-      <c r="O24" s="13">
+      <c r="O24" s="12">
         <v>209.3</v>
       </c>
       <c r="Q24">
@@ -1290,21 +1299,21 @@
       </c>
     </row>
     <row r="25" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G25" s="6">
+      <c r="G25" s="5">
         <v>20150</v>
       </c>
-      <c r="H25" s="7"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="6">
+      <c r="H25" s="6"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="5">
         <v>20150</v>
       </c>
-      <c r="K25" s="7"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="6">
+      <c r="K25" s="6"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="5">
         <v>20150</v>
       </c>
-      <c r="N25" s="7"/>
-      <c r="O25" s="8"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="7"/>
       <c r="Q25">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -1318,8 +1327,91 @@
         <v>0</v>
       </c>
     </row>
+    <row r="27" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="G27" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+    </row>
+    <row r="28" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="G28" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H28" s="20">
+        <v>74176</v>
+      </c>
+      <c r="I28" s="3"/>
+    </row>
+    <row r="29" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="G29" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="H29" s="14">
+        <v>0.14940000000000001</v>
+      </c>
+      <c r="I29" s="16">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="30" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="G30" s="3"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="2"/>
+    </row>
+    <row r="31" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="G31" s="9">
+        <v>9850</v>
+      </c>
+      <c r="H31" s="10">
+        <v>2.0497999999999998</v>
+      </c>
+      <c r="I31" s="12">
+        <v>-16.600000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="G32" s="5">
+        <v>10000</v>
+      </c>
+      <c r="H32" s="6"/>
+      <c r="I32" s="7"/>
+    </row>
+    <row r="33" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G33" s="9">
+        <v>10150</v>
+      </c>
+      <c r="H33" s="10">
+        <v>2.0792199999999998</v>
+      </c>
+      <c r="I33" s="12">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="34" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G34" s="3"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="2"/>
+    </row>
+    <row r="35" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G35" s="9">
+        <v>20000</v>
+      </c>
+      <c r="H35" s="10">
+        <v>5.0856500000000002</v>
+      </c>
+      <c r="I35" s="12">
+        <v>262.3</v>
+      </c>
+    </row>
+    <row r="36" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G36" s="3"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="G27:I27"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="M1:O1"/>

</xml_diff>

<commit_message>
Inductance simulasyonu üzerinde debelenmeceler ve analitik modelleme çalışmaları.
</commit_message>
<xml_diff>
--- a/Simulation/analytical model/harmonic_components.xlsx
+++ b/Simulation/analytical model/harmonic_components.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\immdnew\Simulation\analytical model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitrepos\IMMD\Simulation\analytical model\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -66,8 +66,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -141,7 +142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -184,14 +185,23 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -473,952 +483,961 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:S36"/>
+  <dimension ref="B1:Y36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="25" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C1" s="19" t="s">
+    <row r="1" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="18" t="s">
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18" t="s">
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18" t="s">
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-    </row>
-    <row r="2" spans="3:19" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="3"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+    </row>
+    <row r="2" spans="2:25" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="D2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="3">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3">
         <v>0.5</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="K2" s="3">
+      <c r="H2" s="3"/>
+      <c r="I2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3">
         <v>0.5</v>
       </c>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="N2" s="3">
+      <c r="K2" s="3"/>
+      <c r="L2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="3">
         <v>0.5</v>
       </c>
-      <c r="O2" s="3"/>
-    </row>
-    <row r="3" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C3" s="13" t="s">
+      <c r="N2" s="3"/>
+      <c r="U2" s="23"/>
+      <c r="V2" s="23"/>
+      <c r="W2" s="23"/>
+      <c r="X2" s="23"/>
+      <c r="Y2" s="23"/>
+    </row>
+    <row r="3" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="14">
+      <c r="C3" s="14">
         <v>197</v>
       </c>
-      <c r="E3" s="15">
-        <f>D3/270</f>
+      <c r="D3" s="15">
+        <f>C3/270</f>
         <v>0.72962962962962963</v>
       </c>
-      <c r="F3" s="16">
+      <c r="E3" s="16">
         <v>36.5</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="F3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="14">
+      <c r="G3" s="14">
         <v>0.42249999999999999</v>
       </c>
-      <c r="I3" s="16">
+      <c r="H3" s="16">
         <v>6.5</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="I3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="14">
+      <c r="J3" s="14">
         <v>0.42230000000000001</v>
       </c>
-      <c r="L3" s="16">
+      <c r="K3" s="16">
         <v>246.5</v>
       </c>
-      <c r="M3" s="13" t="s">
+      <c r="L3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="N3" s="14">
+      <c r="M3" s="14">
         <v>0.42220000000000002</v>
       </c>
-      <c r="O3" s="16">
+      <c r="N3" s="16">
         <v>126.5</v>
       </c>
+      <c r="P3">
+        <f>H3-K3</f>
+        <v>-240</v>
+      </c>
       <c r="Q3">
-        <f>I3-L3</f>
-        <v>-240</v>
+        <f>K3-N3</f>
+        <v>120</v>
       </c>
       <c r="R3">
-        <f>L3-O3</f>
+        <f>N3-H3</f>
         <v>120</v>
       </c>
-      <c r="S3">
-        <f>O3-I3</f>
+      <c r="T3" s="21"/>
+    </row>
+    <row r="4" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B4" s="3"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="2"/>
+      <c r="T4" s="21"/>
+    </row>
+    <row r="5" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B5" s="9">
+        <v>9900</v>
+      </c>
+      <c r="C5" s="10">
+        <v>56.4818</v>
+      </c>
+      <c r="D5" s="11">
+        <f>C5/270</f>
+        <v>0.20919185185185185</v>
+      </c>
+      <c r="E5" s="12">
+        <v>103</v>
+      </c>
+      <c r="F5" s="9">
+        <v>9900</v>
+      </c>
+      <c r="G5" s="10">
+        <v>0.1205</v>
+      </c>
+      <c r="H5" s="12">
+        <v>77</v>
+      </c>
+      <c r="I5" s="9">
+        <v>9900</v>
+      </c>
+      <c r="J5" s="10">
+        <v>0.12089999999999999</v>
+      </c>
+      <c r="K5" s="12">
+        <v>-43</v>
+      </c>
+      <c r="L5" s="9">
+        <v>9900</v>
+      </c>
+      <c r="M5" s="10">
+        <v>0.12089999999999999</v>
+      </c>
+      <c r="N5" s="12">
+        <v>196</v>
+      </c>
+      <c r="P5">
+        <f t="shared" ref="P5:P12" si="0">H5-K5</f>
         <v>120</v>
       </c>
-    </row>
-    <row r="4" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C4" s="3"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="2"/>
-    </row>
-    <row r="5" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C5" s="9">
-        <v>9900</v>
-      </c>
-      <c r="D5" s="10">
-        <v>56.4818</v>
-      </c>
-      <c r="E5" s="11">
-        <f>D5/270</f>
-        <v>0.20919185185185185</v>
-      </c>
-      <c r="F5" s="12">
+      <c r="Q5">
+        <f t="shared" ref="Q5:Q12" si="1">K5-N5</f>
+        <v>-239</v>
+      </c>
+      <c r="R5">
+        <f t="shared" ref="R5:R12" si="2">N5-H5</f>
+        <v>119</v>
+      </c>
+      <c r="T5" s="21"/>
+    </row>
+    <row r="6" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B6" s="5">
+        <v>10000</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="5">
+        <v>10000</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0.38569999999999999</v>
+      </c>
+      <c r="H6" s="7">
+        <v>90</v>
+      </c>
+      <c r="I6" s="5">
+        <v>10000</v>
+      </c>
+      <c r="J6" s="6">
+        <v>0.38579999999999998</v>
+      </c>
+      <c r="K6" s="7">
+        <v>90</v>
+      </c>
+      <c r="L6" s="5">
+        <v>10000</v>
+      </c>
+      <c r="M6" s="6">
+        <v>0.38590000000000002</v>
+      </c>
+      <c r="N6" s="7">
+        <v>90</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B7" s="9">
+        <v>10100</v>
+      </c>
+      <c r="C7" s="10">
+        <v>56.4358</v>
+      </c>
+      <c r="D7" s="11">
+        <f>C7/270</f>
+        <v>0.20902148148148147</v>
+      </c>
+      <c r="E7" s="12">
+        <v>69</v>
+      </c>
+      <c r="F7" s="9">
+        <v>10100</v>
+      </c>
+      <c r="G7" s="10">
+        <v>0.1208</v>
+      </c>
+      <c r="H7" s="12">
         <v>103</v>
       </c>
-      <c r="G5" s="9">
-        <v>9900</v>
-      </c>
-      <c r="H5" s="10">
-        <v>0.1205</v>
-      </c>
-      <c r="I5" s="12">
-        <v>77</v>
-      </c>
-      <c r="J5" s="9">
-        <v>9900</v>
-      </c>
-      <c r="K5" s="10">
-        <v>0.12089999999999999</v>
-      </c>
-      <c r="L5" s="12">
-        <v>-43</v>
-      </c>
-      <c r="M5" s="9">
-        <v>9900</v>
-      </c>
-      <c r="N5" s="10">
-        <v>0.12089999999999999</v>
-      </c>
-      <c r="O5" s="12">
-        <v>196</v>
-      </c>
-      <c r="Q5">
-        <f t="shared" ref="Q5:Q12" si="0">I5-L5</f>
-        <v>120</v>
-      </c>
-      <c r="R5">
-        <f t="shared" ref="R5:R12" si="1">L5-O5</f>
-        <v>-239</v>
-      </c>
-      <c r="S5">
-        <f t="shared" ref="S5:S12" si="2">O5-I5</f>
-        <v>119</v>
-      </c>
-    </row>
-    <row r="6" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C6" s="5">
-        <v>10000</v>
-      </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="5">
-        <v>10000</v>
-      </c>
-      <c r="H6" s="6">
-        <v>0.38569999999999999</v>
-      </c>
-      <c r="I6" s="7">
-        <v>90</v>
-      </c>
-      <c r="J6" s="5">
-        <v>10000</v>
-      </c>
-      <c r="K6" s="6">
-        <v>0.38579999999999998</v>
-      </c>
-      <c r="L6" s="7">
-        <v>90</v>
-      </c>
-      <c r="M6" s="5">
-        <v>10000</v>
-      </c>
-      <c r="N6" s="6">
-        <v>0.38590000000000002</v>
-      </c>
-      <c r="O6" s="7">
-        <v>90</v>
-      </c>
-      <c r="Q6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C7" s="9">
+      <c r="I7" s="9">
         <v>10100</v>
       </c>
-      <c r="D7" s="10">
-        <v>56.4358</v>
-      </c>
-      <c r="E7" s="11">
-        <f>D7/270</f>
-        <v>0.20902148148148147</v>
-      </c>
-      <c r="F7" s="12">
-        <v>69</v>
-      </c>
-      <c r="G7" s="9">
+      <c r="J7" s="10">
+        <v>0.1207</v>
+      </c>
+      <c r="K7" s="12">
+        <v>223</v>
+      </c>
+      <c r="L7" s="9">
         <v>10100</v>
       </c>
-      <c r="H7" s="10">
-        <v>0.1208</v>
-      </c>
-      <c r="I7" s="12">
-        <v>103</v>
-      </c>
-      <c r="J7" s="9">
-        <v>10100</v>
-      </c>
-      <c r="K7" s="10">
+      <c r="M7" s="10">
         <v>0.1207</v>
       </c>
-      <c r="L7" s="12">
-        <v>223</v>
-      </c>
-      <c r="M7" s="9">
-        <v>10100</v>
-      </c>
-      <c r="N7" s="10">
-        <v>0.1207</v>
-      </c>
-      <c r="O7" s="12">
+      <c r="N7" s="12">
         <v>-16</v>
       </c>
-      <c r="Q7">
+      <c r="P7">
         <f t="shared" si="0"/>
         <v>-120</v>
       </c>
-      <c r="R7">
+      <c r="Q7">
         <f t="shared" si="1"/>
         <v>239</v>
       </c>
-      <c r="S7">
+      <c r="R7">
         <f t="shared" si="2"/>
         <v>-119</v>
       </c>
     </row>
-    <row r="8" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C8" s="3"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="2"/>
-    </row>
-    <row r="9" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C9" s="5">
+    <row r="8" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B8" s="3"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B9" s="5">
         <v>19850</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="5">
+      <c r="C9" s="6"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="5">
         <v>19850</v>
       </c>
-      <c r="H9" s="6">
+      <c r="G9" s="6">
         <v>7.8299999999999995E-2</v>
       </c>
-      <c r="I9" s="7">
+      <c r="H9" s="7">
         <v>-19</v>
       </c>
-      <c r="J9" s="5">
+      <c r="I9" s="5">
         <v>19850</v>
       </c>
-      <c r="K9" s="6">
+      <c r="J9" s="6">
         <v>7.8399999999999997E-2</v>
       </c>
-      <c r="L9" s="7">
+      <c r="K9" s="7">
         <v>-20</v>
       </c>
-      <c r="M9" s="5">
+      <c r="L9" s="5">
         <v>19850</v>
       </c>
-      <c r="N9" s="6">
+      <c r="M9" s="6">
         <v>7.8100000000000003E-2</v>
       </c>
-      <c r="O9" s="7">
+      <c r="N9" s="7">
         <v>-20</v>
       </c>
-      <c r="Q9">
+      <c r="P9">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="Q9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="R9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S9">
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C10" s="9">
+    <row r="10" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B10" s="9">
         <v>19950</v>
       </c>
-      <c r="D10" s="10">
+      <c r="C10" s="10">
         <v>67.620199999999997</v>
       </c>
-      <c r="E10" s="11">
-        <f>D10/270</f>
+      <c r="D10" s="11">
+        <f>C10/270</f>
         <v>0.25044518518518516</v>
       </c>
-      <c r="F10" s="12">
+      <c r="E10" s="12">
         <v>-43</v>
       </c>
-      <c r="G10" s="9">
+      <c r="F10" s="9">
         <v>19950</v>
       </c>
-      <c r="H10" s="10">
+      <c r="G10" s="10">
         <v>0.14510000000000001</v>
       </c>
-      <c r="I10" s="12">
+      <c r="H10" s="12">
         <v>-6</v>
       </c>
-      <c r="J10" s="9">
+      <c r="I10" s="9">
         <v>19950</v>
       </c>
-      <c r="K10" s="10">
+      <c r="J10" s="10">
         <v>0.14480000000000001</v>
       </c>
-      <c r="L10" s="12">
+      <c r="K10" s="12">
         <v>113</v>
       </c>
-      <c r="M10" s="9">
+      <c r="L10" s="9">
         <v>19950</v>
       </c>
-      <c r="N10" s="10">
+      <c r="M10" s="10">
         <v>0.14480000000000001</v>
       </c>
-      <c r="O10" s="12">
+      <c r="N10" s="12">
         <v>233</v>
       </c>
-      <c r="Q10">
+      <c r="P10">
         <f t="shared" si="0"/>
         <v>-119</v>
       </c>
-      <c r="R10">
+      <c r="Q10">
         <f t="shared" si="1"/>
         <v>-120</v>
       </c>
-      <c r="S10">
+      <c r="R10">
         <f t="shared" si="2"/>
         <v>239</v>
       </c>
     </row>
-    <row r="11" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C11" s="9">
+    <row r="11" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B11" s="9">
         <v>20050</v>
       </c>
-      <c r="D11" s="10">
+      <c r="C11" s="10">
         <v>67.704899999999995</v>
       </c>
-      <c r="E11" s="11">
-        <f>D11/270</f>
+      <c r="D11" s="11">
+        <f>C11/270</f>
         <v>0.25075888888888886</v>
       </c>
-      <c r="F11" s="12">
+      <c r="E11" s="12">
         <v>209</v>
       </c>
-      <c r="G11" s="9">
+      <c r="F11" s="9">
         <v>20050</v>
       </c>
-      <c r="H11" s="10">
+      <c r="G11" s="10">
         <v>0.14480000000000001</v>
       </c>
-      <c r="I11" s="12">
+      <c r="H11" s="12">
         <v>186</v>
       </c>
-      <c r="J11" s="9">
+      <c r="I11" s="9">
         <v>20050</v>
       </c>
-      <c r="K11" s="10">
+      <c r="J11" s="10">
         <v>0.14499999999999999</v>
       </c>
-      <c r="L11" s="12">
+      <c r="K11" s="12">
         <v>67</v>
       </c>
-      <c r="M11" s="9">
+      <c r="L11" s="9">
         <v>20050</v>
       </c>
-      <c r="N11" s="10">
+      <c r="M11" s="10">
         <v>0.14499999999999999</v>
       </c>
-      <c r="O11" s="12">
+      <c r="N11" s="12">
         <v>-53</v>
       </c>
-      <c r="Q11">
+      <c r="P11">
         <f t="shared" si="0"/>
         <v>119</v>
       </c>
-      <c r="R11">
+      <c r="Q11">
         <f t="shared" si="1"/>
         <v>120</v>
       </c>
-      <c r="S11">
+      <c r="R11">
         <f t="shared" si="2"/>
         <v>-239</v>
       </c>
     </row>
-    <row r="12" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C12" s="5">
+    <row r="12" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B12" s="5">
         <v>20150</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="5">
+      <c r="C12" s="6"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="5">
         <v>20150</v>
       </c>
-      <c r="H12" s="6">
+      <c r="G12" s="6">
         <v>7.85E-2</v>
       </c>
-      <c r="I12" s="7">
+      <c r="H12" s="7">
         <v>199</v>
       </c>
-      <c r="J12" s="5">
+      <c r="I12" s="5">
         <v>20150</v>
       </c>
-      <c r="K12" s="6">
+      <c r="J12" s="6">
         <v>7.8299999999999995E-2</v>
       </c>
-      <c r="L12" s="7">
+      <c r="K12" s="7">
         <v>199</v>
       </c>
-      <c r="M12" s="5">
+      <c r="L12" s="5">
         <v>20150</v>
       </c>
-      <c r="N12" s="6">
+      <c r="M12" s="6">
         <v>7.8100000000000003E-2</v>
       </c>
-      <c r="O12" s="7">
+      <c r="N12" s="7">
         <v>199</v>
       </c>
+      <c r="P12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="Q12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="G14" s="18" t="s">
+    <row r="14" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="F14" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18" t="s">
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18" t="s">
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="N14" s="18"/>
-      <c r="O14" s="18"/>
-    </row>
-    <row r="15" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="G15" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
+    </row>
+    <row r="15" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="F15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" s="3"/>
       <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="I15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J15" s="3"/>
       <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="L15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="M15" s="3"/>
       <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-    </row>
-    <row r="16" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="G16" s="13" t="s">
+    </row>
+    <row r="16" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="F16" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="H16" s="14">
+      <c r="G16" s="14">
         <v>11.744199999999999</v>
       </c>
-      <c r="I16" s="16">
+      <c r="H16" s="16">
         <v>-0.8</v>
       </c>
-      <c r="J16" s="13" t="s">
+      <c r="I16" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K16" s="14">
+      <c r="J16" s="14">
         <v>11.7676</v>
       </c>
-      <c r="L16" s="16">
+      <c r="K16" s="16">
         <v>239.7</v>
       </c>
-      <c r="M16" s="13" t="s">
+      <c r="L16" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="N16" s="14">
+      <c r="M16" s="14">
         <v>11.8529</v>
       </c>
-      <c r="O16" s="16">
+      <c r="N16" s="16">
         <v>119.3</v>
       </c>
+      <c r="P16">
+        <f>H16-K16</f>
+        <v>-240.5</v>
+      </c>
       <c r="Q16">
-        <f>I16-L16</f>
-        <v>-240.5</v>
+        <f>K16-N16</f>
+        <v>120.39999999999999</v>
       </c>
       <c r="R16">
-        <f>L16-O16</f>
-        <v>120.39999999999999</v>
-      </c>
-      <c r="S16">
-        <f>O16-I16</f>
+        <f>N16-H16</f>
         <v>120.1</v>
       </c>
     </row>
-    <row r="17" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G17" s="3"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="2"/>
-    </row>
-    <row r="18" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G18" s="9">
+    <row r="17" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="F17" s="3"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="2"/>
+    </row>
+    <row r="18" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="F18" s="9">
         <v>9900</v>
       </c>
-      <c r="H18" s="10">
+      <c r="G18" s="10">
         <v>0.14949999999999999</v>
       </c>
-      <c r="I18" s="12">
+      <c r="H18" s="12">
         <v>-16.600000000000001</v>
       </c>
-      <c r="J18" s="9">
+      <c r="I18" s="9">
         <v>9900</v>
       </c>
-      <c r="K18" s="10">
+      <c r="J18" s="10">
         <v>0.14990000000000001</v>
       </c>
-      <c r="L18" s="12">
+      <c r="K18" s="12">
         <v>223.3</v>
       </c>
-      <c r="M18" s="9">
+      <c r="L18" s="9">
         <v>9900</v>
       </c>
-      <c r="N18" s="10">
+      <c r="M18" s="10">
         <v>0.1497</v>
       </c>
-      <c r="O18" s="12">
+      <c r="N18" s="12">
         <v>103.3</v>
       </c>
+      <c r="P18">
+        <f t="shared" ref="P18:P20" si="3">H18-K18</f>
+        <v>-239.9</v>
+      </c>
       <c r="Q18">
-        <f t="shared" ref="Q18:Q20" si="3">I18-L18</f>
-        <v>-239.9</v>
+        <f t="shared" ref="Q18:Q20" si="4">K18-N18</f>
+        <v>120.00000000000001</v>
       </c>
       <c r="R18">
-        <f t="shared" ref="R18:R20" si="4">L18-O18</f>
-        <v>120.00000000000001</v>
-      </c>
-      <c r="S18">
-        <f t="shared" ref="S18:S20" si="5">O18-I18</f>
+        <f t="shared" ref="R18:R20" si="5">N18-H18</f>
         <v>119.9</v>
       </c>
     </row>
-    <row r="19" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G19" s="5">
+    <row r="19" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="F19" s="5">
         <v>10000</v>
       </c>
-      <c r="H19" s="6"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="5">
+      <c r="G19" s="6"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="5">
         <v>10000</v>
       </c>
-      <c r="K19" s="6"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="5">
+      <c r="J19" s="6"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="5">
         <v>10000</v>
       </c>
-      <c r="N19" s="6"/>
-      <c r="O19" s="7"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="7"/>
+      <c r="P19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Q19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="R19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="S19">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G20" s="9">
+    <row r="20" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="F20" s="9">
         <v>10100</v>
       </c>
-      <c r="H20" s="10">
+      <c r="G20" s="10">
         <v>0.14680000000000001</v>
       </c>
-      <c r="I20" s="12">
+      <c r="H20" s="12">
         <v>9.5</v>
       </c>
-      <c r="J20" s="9">
+      <c r="I20" s="9">
         <v>10100</v>
       </c>
-      <c r="K20" s="10">
+      <c r="J20" s="10">
         <v>0.14660000000000001</v>
       </c>
-      <c r="L20" s="12">
+      <c r="K20" s="12">
         <v>129.4</v>
       </c>
-      <c r="M20" s="9">
+      <c r="L20" s="9">
         <v>10100</v>
       </c>
-      <c r="N20" s="10">
+      <c r="M20" s="10">
         <v>0.14680000000000001</v>
       </c>
-      <c r="O20" s="12">
+      <c r="N20" s="12">
         <v>249.4</v>
       </c>
-      <c r="Q20">
+      <c r="P20">
         <f t="shared" si="3"/>
         <v>-119.9</v>
       </c>
-      <c r="R20">
+      <c r="Q20">
         <f t="shared" si="4"/>
         <v>-120</v>
       </c>
-      <c r="S20">
+      <c r="R20">
         <f t="shared" si="5"/>
         <v>239.9</v>
       </c>
     </row>
-    <row r="21" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G21" s="3"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="2"/>
-    </row>
-    <row r="22" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G22" s="5">
+    <row r="21" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="F21" s="3"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="2"/>
+    </row>
+    <row r="22" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="F22" s="5">
         <v>19850</v>
       </c>
-      <c r="H22" s="6"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="5">
+      <c r="G22" s="6"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="5">
         <v>19850</v>
       </c>
-      <c r="K22" s="6"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="5">
+      <c r="J22" s="6"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="5">
         <v>19850</v>
       </c>
-      <c r="N22" s="6"/>
-      <c r="O22" s="7"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="7"/>
+      <c r="P22">
+        <f t="shared" ref="P22:P25" si="6">H22-K22</f>
+        <v>0</v>
+      </c>
       <c r="Q22">
-        <f t="shared" ref="Q22:Q25" si="6">I22-L22</f>
+        <f t="shared" ref="Q22:Q25" si="7">K22-N22</f>
         <v>0</v>
       </c>
       <c r="R22">
-        <f t="shared" ref="R22:R25" si="7">L22-O22</f>
-        <v>0</v>
-      </c>
-      <c r="S22">
-        <f t="shared" ref="S22:S25" si="8">O22-I22</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G23" s="9">
+        <f t="shared" ref="R22:R25" si="8">N22-H22</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="F23" s="9">
         <v>19950</v>
       </c>
-      <c r="H23" s="10">
+      <c r="G23" s="10">
         <v>8.9200000000000002E-2</v>
       </c>
-      <c r="I23" s="12">
+      <c r="H23" s="12">
         <v>256</v>
       </c>
-      <c r="J23" s="9">
+      <c r="I23" s="9">
         <v>19950</v>
       </c>
-      <c r="K23" s="10">
+      <c r="J23" s="10">
         <v>8.8900000000000007E-2</v>
       </c>
-      <c r="L23" s="12">
+      <c r="K23" s="12">
         <v>16.2</v>
       </c>
-      <c r="M23" s="9">
+      <c r="L23" s="9">
         <v>19950</v>
       </c>
-      <c r="N23" s="10">
+      <c r="M23" s="10">
         <v>8.9200000000000002E-2</v>
       </c>
-      <c r="O23" s="12">
+      <c r="N23" s="12">
         <v>136.1</v>
       </c>
-      <c r="Q23">
+      <c r="P23">
         <f t="shared" si="6"/>
         <v>239.8</v>
       </c>
-      <c r="R23">
+      <c r="Q23">
         <f t="shared" si="7"/>
         <v>-119.89999999999999</v>
       </c>
-      <c r="S23">
+      <c r="R23">
         <f t="shared" si="8"/>
         <v>-119.9</v>
       </c>
     </row>
-    <row r="24" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G24" s="9">
+    <row r="24" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="F24" s="9">
         <v>20050</v>
       </c>
-      <c r="H24" s="10">
+      <c r="G24" s="10">
         <v>8.8599999999999998E-2</v>
       </c>
-      <c r="I24" s="12">
+      <c r="H24" s="12">
         <v>89</v>
       </c>
-      <c r="J24" s="9">
+      <c r="I24" s="9">
         <v>20050</v>
       </c>
-      <c r="K24" s="10">
+      <c r="J24" s="10">
         <v>8.8599999999999998E-2</v>
       </c>
-      <c r="L24" s="12">
+      <c r="K24" s="12">
         <v>-30.6</v>
       </c>
-      <c r="M24" s="9">
+      <c r="L24" s="9">
         <v>20050</v>
       </c>
-      <c r="N24" s="10">
+      <c r="M24" s="10">
         <v>8.8700000000000001E-2</v>
       </c>
-      <c r="O24" s="12">
+      <c r="N24" s="12">
         <v>209.3</v>
       </c>
-      <c r="Q24">
+      <c r="P24">
         <f t="shared" si="6"/>
         <v>119.6</v>
       </c>
-      <c r="R24">
+      <c r="Q24">
         <f t="shared" si="7"/>
         <v>-239.9</v>
       </c>
-      <c r="S24">
+      <c r="R24">
         <f t="shared" si="8"/>
         <v>120.30000000000001</v>
       </c>
     </row>
-    <row r="25" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G25" s="5">
+    <row r="25" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="F25" s="5">
         <v>20150</v>
       </c>
-      <c r="H25" s="6"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="5">
+      <c r="G25" s="6"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="5">
         <v>20150</v>
       </c>
-      <c r="K25" s="6"/>
-      <c r="L25" s="7"/>
-      <c r="M25" s="5">
+      <c r="J25" s="6"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="5">
         <v>20150</v>
       </c>
-      <c r="N25" s="6"/>
-      <c r="O25" s="7"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="7"/>
+      <c r="P25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="Q25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="R25">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="S25">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G27" s="18" t="s">
+    <row r="27" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="F27" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-    </row>
-    <row r="28" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G28" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H28" s="20">
-        <v>74176</v>
-      </c>
-      <c r="I28" s="3"/>
-    </row>
-    <row r="29" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G29" s="13" t="s">
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+    </row>
+    <row r="28" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="F28" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G28" s="18">
+        <v>7.4176000000000002</v>
+      </c>
+      <c r="H28" s="3"/>
+    </row>
+    <row r="29" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="F29" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="H29" s="14">
+      <c r="G29" s="14">
         <v>0.14940000000000001</v>
       </c>
-      <c r="I29" s="16">
+      <c r="H29" s="16">
         <v>125</v>
       </c>
     </row>
-    <row r="30" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G30" s="3"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="2"/>
-    </row>
-    <row r="31" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G31" s="9">
+    <row r="30" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="F30" s="3"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="F31" s="9">
         <v>9850</v>
       </c>
-      <c r="H31" s="10">
+      <c r="G31" s="10">
         <v>2.0497999999999998</v>
       </c>
-      <c r="I31" s="12">
+      <c r="H31" s="12">
         <v>-16.600000000000001</v>
       </c>
     </row>
-    <row r="32" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G32" s="5">
+    <row r="32" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="F32" s="5">
         <v>10000</v>
       </c>
-      <c r="H32" s="6"/>
-      <c r="I32" s="7"/>
-    </row>
-    <row r="33" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G33" s="9">
+      <c r="G32" s="6"/>
+      <c r="H32" s="7"/>
+    </row>
+    <row r="33" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F33" s="9">
         <v>10150</v>
       </c>
-      <c r="H33" s="10">
+      <c r="G33" s="10">
         <v>2.0792199999999998</v>
       </c>
-      <c r="I33" s="12">
+      <c r="H33" s="12">
         <v>5.4</v>
       </c>
     </row>
-    <row r="34" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G34" s="3"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="2"/>
-    </row>
-    <row r="35" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G35" s="9">
+    <row r="34" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F34" s="3"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="2"/>
+    </row>
+    <row r="35" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F35" s="9">
         <v>20000</v>
       </c>
-      <c r="H35" s="10">
+      <c r="G35" s="10">
         <v>5.0856500000000002</v>
       </c>
-      <c r="I35" s="12">
+      <c r="H35" s="12">
         <v>262.3</v>
       </c>
     </row>
-    <row r="36" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G36" s="3"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="2"/>
+    <row r="36" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F36" s="3"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="L14:N14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
DC bara analitik modellemesi üzerine kapsamılı bir çalışma yapıldı. Simulasyon modeli çalışır hale getirildi. Interleaving etkileri detaylı olarak incelendi.
</commit_message>
<xml_diff>
--- a/Simulation/analytical model/harmonic_components.xlsx
+++ b/Simulation/analytical model/harmonic_components.xlsx
@@ -66,9 +66,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="165" formatCode="#,##0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -89,7 +88,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -111,6 +110,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -142,7 +147,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -185,8 +190,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -194,14 +205,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -483,40 +497,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:Y36"/>
+  <dimension ref="B1:Y42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="25" width="9.140625" style="22"/>
+    <col min="21" max="25" width="9.140625" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="19" t="s">
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19" t="s">
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19" t="s">
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
     </row>
     <row r="2" spans="2:25" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="3"/>
@@ -548,11 +562,11 @@
         <v>0.5</v>
       </c>
       <c r="N2" s="3"/>
-      <c r="U2" s="23"/>
-      <c r="V2" s="23"/>
-      <c r="W2" s="23"/>
-      <c r="X2" s="23"/>
-      <c r="Y2" s="23"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="20"/>
+      <c r="X2" s="20"/>
+      <c r="Y2" s="20"/>
     </row>
     <row r="3" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
@@ -607,7 +621,7 @@
         <f>N3-H3</f>
         <v>120</v>
       </c>
-      <c r="T3" s="21"/>
+      <c r="T3" s="18"/>
     </row>
     <row r="4" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
@@ -623,7 +637,7 @@
       <c r="L4" s="3"/>
       <c r="M4" s="4"/>
       <c r="N4" s="2"/>
-      <c r="T4" s="21"/>
+      <c r="T4" s="18"/>
     </row>
     <row r="5" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B5" s="9">
@@ -678,7 +692,7 @@
         <f t="shared" ref="R5:R12" si="2">N5-H5</f>
         <v>119</v>
       </c>
-      <c r="T5" s="21"/>
+      <c r="T5" s="18"/>
     </row>
     <row r="6" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B6" s="5">
@@ -999,21 +1013,21 @@
       </c>
     </row>
     <row r="14" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="F14" s="19" t="s">
+      <c r="F14" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19" t="s">
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="19" t="s">
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="M14" s="19"/>
-      <c r="N14" s="19"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
     </row>
     <row r="15" spans="2:25" x14ac:dyDescent="0.25">
       <c r="F15" s="3" t="s">
@@ -1347,17 +1361,17 @@
       </c>
     </row>
     <row r="27" spans="6:18" x14ac:dyDescent="0.25">
-      <c r="F27" s="19" t="s">
+      <c r="F27" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
     </row>
     <row r="28" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F28" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G28" s="18">
+      <c r="G28" s="24">
         <v>7.4176000000000002</v>
       </c>
       <c r="H28" s="3"/>
@@ -1427,6 +1441,56 @@
       <c r="F36" s="3"/>
       <c r="G36" s="4"/>
       <c r="H36" s="2"/>
+    </row>
+    <row r="37" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F37" s="9">
+        <v>29850</v>
+      </c>
+      <c r="G37" s="25">
+        <v>0.41277700000000001</v>
+      </c>
+      <c r="H37" s="9"/>
+    </row>
+    <row r="38" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F38" s="9">
+        <v>30150</v>
+      </c>
+      <c r="G38" s="25">
+        <v>0.49381900000000001</v>
+      </c>
+      <c r="H38" s="9"/>
+    </row>
+    <row r="39" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F39" s="23"/>
+      <c r="G39" s="26"/>
+      <c r="H39" s="23"/>
+    </row>
+    <row r="40" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F40" s="9">
+        <v>39700</v>
+      </c>
+      <c r="G40" s="25">
+        <v>0.64641899999999997</v>
+      </c>
+      <c r="H40" s="9"/>
+    </row>
+    <row r="41" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F41" s="9">
+        <v>40000</v>
+      </c>
+      <c r="G41" s="25">
+        <v>1.9245099999999999</v>
+      </c>
+      <c r="H41" s="9"/>
+    </row>
+    <row r="42" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F42" s="9">
+        <v>40300</v>
+      </c>
+      <c r="G42" s="25">
+        <v>0.66368400000000005</v>
+      </c>
+      <c r="H42" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>